<commit_message>
decompose the input variables and add shuffle data
</commit_message>
<xml_diff>
--- a/LCA/LCA_CO2.xlsx
+++ b/LCA/LCA_CO2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ranjing/Desktop/ML_US_ENERGY/LCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC82DF0-FB6E-3846-9DE7-61633E764217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F490DCB2-BB1C-F84B-B924-56BA7934181F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6D5D55A3-CBE5-594B-8FB8-2678FFA7578F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{6D5D55A3-CBE5-594B-8FB8-2678FFA7578F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
   <si>
     <t>Coal Consumption, Total</t>
   </si>
@@ -560,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,6 +643,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4883,37 +4889,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -5121,6 +5097,28 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-E207-BD42-8EE8-CF91E558E64B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3829027481544441E-2"/>
+                  <c:y val="-6.3054513143840215E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-80C8-3B4F-ADBF-7926DC247D9C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -6571,15 +6569,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1352550</xdr:colOff>
-      <xdr:row>612</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>616</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>635</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>1866900</xdr:colOff>
+      <xdr:row>639</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6904,10 +6902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F1A728-6D1C-AF48-9969-9028282634E5}">
-  <dimension ref="A1:T627"/>
+  <dimension ref="A1:T628"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="113" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="G18" zoomScale="113" workbookViewId="0">
+      <selection activeCell="H18" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -7222,10 +7220,10 @@
       <c r="Q26" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R26" s="31" t="s">
+      <c r="R26" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="S26" s="30" t="s">
+      <c r="S26" s="32" t="s">
         <v>47</v>
       </c>
       <c r="T26" s="21" t="s">
@@ -7282,8 +7280,8 @@
       <c r="Q27" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="R27" s="31"/>
-      <c r="S27" s="30"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="32"/>
       <c r="T27" s="21" t="s">
         <v>45</v>
       </c>
@@ -50487,6 +50485,76 @@
       <c r="T627" s="20">
         <v>454.09100000000001</v>
       </c>
+    </row>
+    <row r="628" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A628" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B628" s="31">
+        <f>SUM(B28:B627)</f>
+        <v>42542576.914000012</v>
+      </c>
+      <c r="C628" s="31">
+        <f>SUM(C28:C627)</f>
+        <v>110695785130.228</v>
+      </c>
+      <c r="D628" s="31">
+        <f>SUM(D28:D627)</f>
+        <v>1124990.0379999997</v>
+      </c>
+      <c r="E628" s="31">
+        <f t="shared" ref="E628:G628" si="100">SUM(E28:E627)</f>
+        <v>61199458067.199913</v>
+      </c>
+      <c r="F628" s="31">
+        <f t="shared" si="100"/>
+        <v>165201405.42399997</v>
+      </c>
+      <c r="G628" s="31">
+        <f t="shared" si="100"/>
+        <v>64098145304.512001</v>
+      </c>
+      <c r="H628" s="31">
+        <f t="shared" ref="H628:Q628" si="101">SUM(H28:H627)</f>
+        <v>487069.65099999972</v>
+      </c>
+      <c r="I628" s="31">
+        <f t="shared" si="101"/>
+        <v>164769282.32087189</v>
+      </c>
+      <c r="J628" s="31">
+        <f t="shared" si="101"/>
+        <v>287101.45799999987</v>
+      </c>
+      <c r="K628" s="31">
+        <f t="shared" si="101"/>
+        <v>97122662.212300152</v>
+      </c>
+      <c r="L628" s="31">
+        <f t="shared" si="101"/>
+        <v>2801731.9720000001</v>
+      </c>
+      <c r="M628" s="31">
+        <f t="shared" si="101"/>
+        <v>952602038.62026811</v>
+      </c>
+      <c r="N628" s="31">
+        <f t="shared" si="101"/>
+        <v>7107041.0979999956</v>
+      </c>
+      <c r="O628" s="31">
+        <f t="shared" si="101"/>
+        <v>2753876794.7872987</v>
+      </c>
+      <c r="P628" s="31">
+        <f t="shared" si="101"/>
+        <v>338919.89400000067</v>
+      </c>
+      <c r="Q628" s="31">
+        <f t="shared" si="101"/>
+        <v>114652160.28958865</v>
+      </c>
+      <c r="T628" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -50502,9 +50570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D5BFC9-1061-8D42-A4B8-E8FE36DC3DEB}">
   <dimension ref="A1:L611"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A610" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A603" sqref="A603:XFD603"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D614" sqref="D614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add check version script
</commit_message>
<xml_diff>
--- a/LCA/LCA_CO2.xlsx
+++ b/LCA/LCA_CO2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ranjing/Desktop/ML_US_ENERGY/LCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52A37CB-42F6-8946-A825-E03EA3B32386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED79B22C-863C-E943-966D-B9597CA6AFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="2" xr2:uid="{6D5D55A3-CBE5-594B-8FB8-2678FFA7578F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{6D5D55A3-CBE5-594B-8FB8-2678FFA7578F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -702,12 +702,6 @@
     <xf numFmtId="11" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -715,6 +709,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5565,6 +5565,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8C79-E447-91E1-8F6395713F87}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -5583,6 +5588,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-8C79-E447-91E1-8F6395713F87}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -5659,6 +5669,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-8C79-E447-91E1-8F6395713F87}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -7560,15 +7575,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4521200</xdr:colOff>
+      <xdr:colOff>4245172</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>253550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3048000</xdr:colOff>
+      <xdr:colOff>2924372</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>147850</xdr:rowOff>
+      <xdr:rowOff>249000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7590,8 +7605,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19507200" y="1790700"/>
-          <a:ext cx="7112000" cy="4503950"/>
+          <a:off x="17529597" y="1894435"/>
+          <a:ext cx="7119642" cy="4558459"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8022,8 +8037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F1A728-6D1C-AF48-9969-9028282634E5}">
   <dimension ref="A1:T628"/>
   <sheetViews>
-    <sheetView topLeftCell="R20" zoomScale="113" workbookViewId="0">
-      <selection activeCell="H18" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="113" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -8338,10 +8353,10 @@
       <c r="Q26" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R26" s="33" t="s">
+      <c r="R26" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="S26" s="32" t="s">
+      <c r="S26" s="35" t="s">
         <v>47</v>
       </c>
       <c r="T26" s="21" t="s">
@@ -8398,8 +8413,8 @@
       <c r="Q27" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="R27" s="33"/>
-      <c r="S27" s="32"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="35"/>
       <c r="T27" s="21" t="s">
         <v>45</v>
       </c>
@@ -51689,7 +51704,7 @@
   <dimension ref="A1:L611"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A613" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A599" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C635" sqref="C635"/>
     </sheetView>
   </sheetViews>
@@ -74732,7 +74747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CC341-8B4E-164D-8966-8CE10D66EA21}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -74750,28 +74765,28 @@
   <sheetData>
     <row r="1" spans="1:10" ht="38" x14ac:dyDescent="0.2">
       <c r="A1" s="17"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="32" t="s">
         <v>65</v>
       </c>
     </row>
@@ -74779,59 +74794,59 @@
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="35">
+      <c r="B2" s="33">
         <v>110695785130.228</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="33">
         <v>61199458067.199913</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="33">
         <v>64098145304.512001</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="33">
         <v>164769282.32087189</v>
       </c>
-      <c r="F2" s="35">
+      <c r="F2" s="33">
         <v>97122662.212300152</v>
       </c>
-      <c r="G2" s="35">
+      <c r="G2" s="33">
         <v>952602038.62026811</v>
       </c>
-      <c r="H2" s="35">
+      <c r="H2" s="33">
         <v>2753876794.7872987</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="33">
         <v>114652160.28958865</v>
       </c>
-      <c r="J2" s="36">
+      <c r="J2" s="34">
         <f>SUM(B2:I2)</f>
         <v>240076411440.17023</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="38" x14ac:dyDescent="0.2">
       <c r="A3" s="17"/>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="32" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change t-test toMann-Whitney U Statistic“
</commit_message>
<xml_diff>
--- a/LCA/LCA_CO2.xlsx
+++ b/LCA/LCA_CO2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ranjing/Desktop/ML_US_ENERGY/LCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7F768C-A745-9C4D-BA8F-158BC4C4CFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5079C30D-408F-FD4B-B08F-B8D56FD99E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="2" xr2:uid="{6D5D55A3-CBE5-594B-8FB8-2678FFA7578F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{6D5D55A3-CBE5-594B-8FB8-2678FFA7578F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -709,13 +709,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8038,8 +8038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F1A728-6D1C-AF48-9969-9028282634E5}">
   <dimension ref="A1:T628"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="113" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -8354,10 +8354,10 @@
       <c r="Q26" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R26" s="36" t="s">
+      <c r="R26" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="S26" s="35" t="s">
+      <c r="S26" s="36" t="s">
         <v>47</v>
       </c>
       <c r="T26" s="21" t="s">
@@ -8414,8 +8414,8 @@
       <c r="Q27" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="R27" s="36"/>
-      <c r="S27" s="35"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="36"/>
       <c r="T27" s="21" t="s">
         <v>45</v>
       </c>
@@ -51704,8 +51704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D5BFC9-1061-8D42-A4B8-E8FE36DC3DEB}">
   <dimension ref="A1:L611"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A624" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D649" sqref="D649"/>
     </sheetView>
   </sheetViews>
@@ -74751,7 +74751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CC341-8B4E-164D-8966-8CE10D66EA21}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -74893,13 +74893,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E5" s="37"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E6" s="37"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="37"/>
+      <c r="C8" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>